<commit_message>
Added 8 more test cases - eBay
</commit_message>
<xml_diff>
--- a/com.ebay/src/test/resources/ebayTestData.xlsx
+++ b/com.ebay/src/test/resources/ebayTestData.xlsx
@@ -8,25 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janna\IdeaProjects\Team1BootCamp\com.ebay\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0200DA-71E6-4AC6-B1E4-5422FCDDC6F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A1B09E-AADF-48CF-9894-5B35F57489FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6855" yWindow="4215" windowWidth="18435" windowHeight="11385" activeTab="3" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
   </bookViews>
   <sheets>
     <sheet name="MostPopularCategories" sheetId="1" r:id="rId1"/>
     <sheet name="MoreCategories" sheetId="2" r:id="rId2"/>
     <sheet name="ShopByCategory" sheetId="3" r:id="rId3"/>
     <sheet name="Search" sheetId="4" r:id="rId4"/>
-    <sheet name="BankOfAmerica" sheetId="5" r:id="rId5"/>
-    <sheet name="BMWUSA" sheetId="6" r:id="rId6"/>
-    <sheet name="Trulia" sheetId="7" r:id="rId7"/>
-    <sheet name="AirBNB" sheetId="8" r:id="rId8"/>
-    <sheet name="OverStock" sheetId="9" r:id="rId9"/>
-    <sheet name="ESPN" sheetId="10" r:id="rId10"/>
-    <sheet name="Verizon" sheetId="11" r:id="rId11"/>
-    <sheet name="Chase" sheetId="12" r:id="rId12"/>
-    <sheet name="Mercedes-Benz" sheetId="13" r:id="rId13"/>
-    <sheet name="Redfin" sheetId="14" r:id="rId14"/>
+    <sheet name="fashionshoeBreadcrumb" sheetId="6" r:id="rId5"/>
+    <sheet name="Breadcrum" sheetId="7" r:id="rId6"/>
+    <sheet name="BuyingFormatList" sheetId="8" r:id="rId7"/>
+    <sheet name="Condtion" sheetId="9" r:id="rId8"/>
+    <sheet name="ESPN" sheetId="10" r:id="rId9"/>
+    <sheet name="Verizon" sheetId="11" r:id="rId10"/>
+    <sheet name="Chase" sheetId="12" r:id="rId11"/>
+    <sheet name="Mercedes-Benz" sheetId="13" r:id="rId12"/>
+    <sheet name="Redfin" sheetId="14" r:id="rId13"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,10 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
-  <si>
-    <t>A</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t>Category Name</t>
   </si>
@@ -128,6 +124,57 @@
   </si>
   <si>
     <t>fdbgfhb</t>
+  </si>
+  <si>
+    <t>Fashion That’s Made for You</t>
+  </si>
+  <si>
+    <t>eBay</t>
+  </si>
+  <si>
+    <t>fashionshoeBreadcrumb</t>
+  </si>
+  <si>
+    <t>Clothing, Shoes &amp; Accessories</t>
+  </si>
+  <si>
+    <t>Women</t>
+  </si>
+  <si>
+    <t>FashionBreadcrum</t>
+  </si>
+  <si>
+    <t>All Listings</t>
+  </si>
+  <si>
+    <t>Best Offer</t>
+  </si>
+  <si>
+    <t>Auction</t>
+  </si>
+  <si>
+    <t>BuyingFormatList</t>
+  </si>
+  <si>
+    <t>Buy It Now</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>New with box</t>
+  </si>
+  <si>
+    <t>New without box</t>
+  </si>
+  <si>
+    <t>New with defects</t>
+  </si>
+  <si>
+    <t>Pre-owned</t>
+  </si>
+  <si>
+    <t>Not Specified</t>
   </si>
 </sst>
 </file>
@@ -527,42 +574,42 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -572,7 +619,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2C6DB0C-125D-41E6-B672-3FA74959CDA8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C4F54D1-3917-41AA-9115-54DFB60054C4}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -586,20 +633,6 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C4F54D1-3917-41AA-9115-54DFB60054C4}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71A4ED8F-84C7-4351-B184-022F160E827E}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -613,7 +646,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BD1F144-5BE0-43B5-8C2F-943F03339C79}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -627,7 +660,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C25186B-8AE5-4703-8BDB-6D9F1A2F53C3}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -654,47 +687,47 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -717,57 +750,57 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -779,7 +812,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0464987E-CA86-496F-AFAF-2580C40BA720}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -790,12 +823,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -804,18 +837,39 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB124C4-9CEE-457F-95C0-47C63DA908AF}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5674FF68-7C81-4A9C-99FE-C7E070DBCFFA}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -824,57 +878,138 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5674FF68-7C81-4A9C-99FE-C7E070DBCFFA}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC436034-E141-4F6F-A259-658744C38455}">
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="35.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC436034-E141-4F6F-A259-658744C38455}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F06E338-1C0F-45E0-B136-3FC6897D7CEC}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.85546875" customWidth="1"/>
   </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3A9241A-80CA-47A8-B8A7-CE843E51095C}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2C6DB0C-125D-41E6-B672-3FA74959CDA8}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3A9241A-80CA-47A8-B8A7-CE843E51095C}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added 4 test cases ebay
</commit_message>
<xml_diff>
--- a/com.ebay/src/test/resources/ebayTestData.xlsx
+++ b/com.ebay/src/test/resources/ebayTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janna\IdeaProjects\Team1BootCamp\com.ebay\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A1B09E-AADF-48CF-9894-5B35F57489FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC309CDC-A8A2-4A01-89F6-A2DE570B5997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="9" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
   </bookViews>
   <sheets>
     <sheet name="MostPopularCategories" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,8 @@
     <sheet name="Breadcrum" sheetId="7" r:id="rId6"/>
     <sheet name="BuyingFormatList" sheetId="8" r:id="rId7"/>
     <sheet name="Condtion" sheetId="9" r:id="rId8"/>
-    <sheet name="ESPN" sheetId="10" r:id="rId9"/>
-    <sheet name="Verizon" sheetId="11" r:id="rId10"/>
+    <sheet name="shoeSize" sheetId="10" r:id="rId9"/>
+    <sheet name="Brand" sheetId="11" r:id="rId10"/>
     <sheet name="Chase" sheetId="12" r:id="rId11"/>
     <sheet name="Mercedes-Benz" sheetId="13" r:id="rId12"/>
     <sheet name="Redfin" sheetId="14" r:id="rId13"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="56">
   <si>
     <t>Category Name</t>
   </si>
@@ -175,6 +175,36 @@
   </si>
   <si>
     <t>Not Specified</t>
+  </si>
+  <si>
+    <t>shoeSize</t>
+  </si>
+  <si>
+    <t>Brand</t>
+  </si>
+  <si>
+    <t>adidas</t>
+  </si>
+  <si>
+    <t>Clarks</t>
+  </si>
+  <si>
+    <t>Crocs</t>
+  </si>
+  <si>
+    <t>Michael Kors</t>
+  </si>
+  <si>
+    <t>Nike</t>
+  </si>
+  <si>
+    <t>Skechers</t>
+  </si>
+  <si>
+    <t>Unbranded</t>
+  </si>
+  <si>
+    <t>VANS</t>
   </si>
 </sst>
 </file>
@@ -243,12 +273,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -620,14 +651,60 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C4F54D1-3917-41AA-9115-54DFB60054C4}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -958,7 +1035,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3A9241A-80CA-47A8-B8A7-CE843E51095C}">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1002,14 +1079,61 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2C6DB0C-125D-41E6-B672-3FA74959CDA8}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added some test cases - ebay
</commit_message>
<xml_diff>
--- a/com.ebay/src/test/resources/ebayTestData.xlsx
+++ b/com.ebay/src/test/resources/ebayTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janna\IdeaProjects\Team1BootCamp\com.ebay\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E663BC4A-EECF-4D89-9F4E-05F8D70816E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FAC89BD-7C81-404A-ACAB-528C068FC53C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="11" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="14" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
   </bookViews>
   <sheets>
     <sheet name="MostPopularCategories" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,9 @@
     <sheet name="Brand" sheetId="11" r:id="rId10"/>
     <sheet name="color" sheetId="12" r:id="rId11"/>
     <sheet name="UpperMaterial" sheetId="13" r:id="rId12"/>
-    <sheet name="Redfin" sheetId="14" r:id="rId13"/>
+    <sheet name="TestCases" sheetId="14" r:id="rId13"/>
+    <sheet name="Price" sheetId="15" r:id="rId14"/>
+    <sheet name="Heel" sheetId="16" r:id="rId15"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="91">
   <si>
     <t>Category Name</t>
   </si>
@@ -265,6 +267,51 @@
   </si>
   <si>
     <t>Plastic</t>
+  </si>
+  <si>
+    <t>TestCase</t>
+  </si>
+  <si>
+    <t>ExpectedResult</t>
+  </si>
+  <si>
+    <t>List View</t>
+  </si>
+  <si>
+    <t>Grid View</t>
+  </si>
+  <si>
+    <t>Gallery View</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Under $20.00</t>
+  </si>
+  <si>
+    <t>$20.00 to $40.00</t>
+  </si>
+  <si>
+    <t>Over $40.00</t>
+  </si>
+  <si>
+    <t>Flat (Under 1 in)</t>
+  </si>
+  <si>
+    <t>High (3-3.9 in)</t>
+  </si>
+  <si>
+    <t>Low (1-1.9 in)</t>
+  </si>
+  <si>
+    <t>Mid (2-2.9 in)</t>
+  </si>
+  <si>
+    <t>Ultra High (4 in &amp; Higher)</t>
+  </si>
+  <si>
+    <t>Heel Height</t>
   </si>
 </sst>
 </file>
@@ -843,7 +890,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BD1F144-5BE0-43B5-8C2F-943F03339C79}">
   <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -902,14 +949,130 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C25186B-8AE5-4703-8BDB-6D9F1A2F53C3}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="33" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C85B0702-9ED7-4780-BA6F-61470C23AE6A}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32B7FDE3-29B1-459A-86BE-DE8EC5333D1D}">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>